<commit_message>
implementation of deliver summary
</commit_message>
<xml_diff>
--- a/web/material/template/deliver_summary_template.xlsx
+++ b/web/material/template/deliver_summary_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wxd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Documents/Itellij/Selling/web/material/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17660" yWindow="4860" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="4460" yWindow="2320" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>发货单号</t>
     <rPh sb="0" eb="1">
@@ -112,6 +112,9 @@
       <t>bei zhu</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快递单号</t>
   </si>
 </sst>
 </file>
@@ -122,14 +125,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -155,11 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -434,43 +440,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>